<commit_message>
Get daily reddit data: Tue Apr 30 08:08:45 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_05.xlsx
+++ b/data/2024_05_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C460"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2709 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1cgn8t7</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Mermaid-ish nails</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c7zsxy6znkxc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1cgm7fs</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Teddy bee nail art</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aw9zbsa7bkxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1cglvl2</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Nails ideas?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pww3ql7a7kxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1cgkhp9</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Match Cherry Dr Pepper can with Cirque Verdigris </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yn8ru3j5sjxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1cgkdir</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>suggestions for wide press on nails</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgkdir/suggestions_for_wide_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1cgk1mu</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>My summer nails 🌼🥹💅🏻</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jom7dbtsnjxc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1cgjqih</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Does anyone else not really like gel x?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgjqih/does_anyone_else_not_really_like_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1cgjd0w</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Decided to do smth different with my natural nails</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m51uvqx3hjxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1cgjaw1</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Hello 👋🏻 I'm planning on making my first press-on nails using Makartt's products, and I have questions (I never do my own manicures before, so I'm excited and worried): 👇🏻 *The questions is in the comment section</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgjaw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1cgj8or</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am in love with a fresh long set </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h40v87cyfjxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1cgh3ii</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Adhesive tab users - how do you shower?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgh3ii/adhesive_tab_users_how_do_you_shower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1cgg0ba</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Is this normal for nail removal?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgg0ba</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1cgfza2</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Amen everyone , stay blessed 🪽</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmsxwnf4nixc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1cfx45l</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Strawberry season 🍓</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfx45l</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1cfwfip</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Did my nails today</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfwfip</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1cgiivn</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>In love with these custom gel press ons🌟✨</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0652y189jxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1cgigz5</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Can I even out the length of my nails without making them disproportionate?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nvswzy0p8jxc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1cgi1wm</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Blingy shorties</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmen51o15jxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1cghsmi</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Life’s too short not to have fun with your nails</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cghsmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1cghm03</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>[UPDATE] Is this normal? I got my nails done for the first time and they look awful to me</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cghm03</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1cghboj</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>{PR} Fairy wings</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cghboj</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1cggrug</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>My Press-Ons for a Concert 💚</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzbrhznvtixc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1cgghct</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Flower nails</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgghct</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1cggbtv</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>current set🫶🏻</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tguuuap1qixc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1cgfjfs</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Nail Prep for Gel</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgfjfs/nail_prep_for_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1cgf0fr</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Sailor Moon birthday nails!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyzsc0c6fixc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1cgelrp</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>My new set of nails</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgelrp</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1cgejmu</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Van Gogh and Picasso</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgejmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1cgehs7</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Sanrio Milk 🥛 Nails 🙂</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgehs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1cgefcs</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>My new set of nails</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgefcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1cge4qy</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Green flash</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cge4qy</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1cge01j</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>new set 😌</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/su1w4wg27ixc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1cgdsqd</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need to refill the acrílica but I wanted to try this polish already </t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrgr113g5ixc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1cfs8qr</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>French tip inspired, but make it floral</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfb3jdzq4dxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1cfr2kb</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Where can I purchase a similar chrome powder(USA) Inspo from @nail_banago on IG</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cfr2kb/where_can_i_purchase_a_similar_chrome_powderusa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1cgc8yb</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Are these okay or am I overreacting?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgc8yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1cgce1g</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Adult nail biter needing help</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgce1g/adult_nail_biter_needing_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1cgcbfw</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Looking to get a manicure with clear coat I’m a male do I use regular clear polish or clear gel polish?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgcbfw/looking_to_get_a_manicure_with_clear_coat_im_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1cgbt4t</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Any Advice on How to Grow Long Strong Nails?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dv9s4hoqhxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1cgb7ls</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>I tried a different shape, which do you think is better, 1 or 2?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgb7ls</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1cgamu2</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Should I be charged for gel nail polish if I brought my own?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgamu2/should_i_be_charged_for_gel_nail_polish_if_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1cgad3s</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>April-Birthmonth/birthday nails</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3i14fihcghxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1cga3sn</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Gel X pop off set</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/459g57ckehxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1cga1dr</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Palate Cleanser Set 🤗 my builder sets arent hitting like I want to. I love a curved square, I’m wondering if I should taper it maybe?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09d53a84ehxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1cg9ojz</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little shimmer for myself </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ys6vrnlbhxc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1cg90oa</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Custom Set from a Friend</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0du1cakz6hxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1cg8b0f</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Glossy wine red 🍷</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwqdsv1y1hxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1cg87mb</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Finally getting into nail art</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg87mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1cg7rey</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Nails for the month of April ✨</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg7rey</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1cg7qzs</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>My New Set 💓</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e37hljtzxgxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1cg7qc4</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>First time I think I did an ok job on my nails that wasn't just a coat of paint.</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivgoiayuxgxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1cg77sg</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>First Attempt At Lava Lamp Nail</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g4db9an8ugxc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1cg723b</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>fall vibes</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukzyw3m3tgxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1cg6u2n</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>We need more jewelry!</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg6u2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1cg6pmj</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>In Japan, I tried the Canmake brand and I’m lowkey obsessed. It applied so easy~</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/euvp2d4mqgxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1cg6a78</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Did these a week ago</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg6a78</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1cg5yh1</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Flower tips for spring</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c76kdlpclgxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1cg5xde</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>so proud</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vq9w4ch4lgxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1cg5jo1</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>First time doing chrome nails🥰</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhd1q83iigxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1cg5eln</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Made this Press-on set for a friend and I love it so much!!!</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg5eln</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1cg56tt</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Essie Vanity Fairest powder dupe?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cg56tt/essie_vanity_fairest_powder_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1cg52am</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>really into minimalist nails lately</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg52am</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1cg4xv3</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>After playing sally face I decided to paint them on a press on nail 😌 would do a full set but other things to paint 🤗</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8tm996m7egxc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1cg4qqh</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>A few sets that happened recently</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg4qqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1cg4jcc</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>first ever gel x set!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg4jcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1cg42tq</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love the flowers </t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3y26mpn18gxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1cg3e05</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>first time doing gel x! any advice appreciated</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ay07vfx23gxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1cg39cf</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Actual heartbreak </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m81kkyo42gxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1cg0r5b</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Broke my beautiful nail </t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hna49kvwjfxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1cg0nwi</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>First time ombre</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tktwese8jfxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1cfzs8z</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>New nail tech jackpot</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfzs8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1cfza0o</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Springtime set</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jzw20qm8fxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1cfz7xp</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>I think this my best set so far!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kwli5y58fxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1cfywe7</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>is it common for acrylics to pop off between fills?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cfywe7/is_it_common_for_acrylics_to_pop_off_between_fills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1cfyten</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Does this color suit me?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfyten</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1cfxhky</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>This is more than two weeks of growth 🥲</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xwxucx7texc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1cfx0dp</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>💚🤍</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfx0dp</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1cfwzr5</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>One of my first ever nails as I’m slowly accepting myself :) made it for birthday</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfwzr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1cfw29j</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Which color suits me the best?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfw29j</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1cfvop8</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manucurist - good low maintenance option? </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otlucmktaexc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1cfvn5l</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Best gel nails I ever had 🌸 Budapest</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfvn5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1cfuyod</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>My most recent practice on myself</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfuyod</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1cfurew</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>New gel nails (done in Madrid) 💅🏻</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5393vqrzdxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1cfuk7o</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye is my favorite !!! </t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2o2tsxaxdxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1cfue2d</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to painting nails </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnswxcfbvdxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1cfu14v</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Spring nails 🌸</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mr2be0msqdxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1cgmvlc</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Thought you guys might appreciate this! The bottle cracked and then my cat knocked it over. It is very firmly stuck 😂😂</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgf2ag69jkxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1cgmsij</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail tech hurt my nail in november 2023, fast forward to april 2024 and my nail still hurts if i press it </t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cgmsij/nail_tech_hurt_my_nail_in_november_2023_fast/</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1cglirx</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Cirque Colours- Mai Mai</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/edu2vh0b3kxc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1cgkr2f</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Is it bad for you, if you do your nails constantly?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cgkr2f/is_it_bad_for_you_if_you_do_your_nails_constantly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1cgkd9g</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Caved and got ILNP Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yk6h70yqjxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1cgk7d9</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Definitely sold on Mooncat!</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgk7d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1cgk4ul</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Stardew Valley summer nails!🐮🌻</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fvefl7nojxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1cgiila</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Armadillos night out</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cxfv26z39jxc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1cgif1c</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Sparkle Cherries✨🍒 💖</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/core4px08jxc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1cgie4c</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Swatch sheet</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srzk8g438jxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1cghm1x</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Dashing Diva ‘Titanium glaze’ and ‘White Syrup’ gel strips</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iurzfi651jxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1cgg0vm</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Any love for those trying to quit biting and picking their nails? One week completed so far! Despite them being short, I’m loving the clean look and can’t wait for more progress.</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ry5fw0uhnixc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1cgfyfe</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>beaux reves: Girl Talk</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgfyfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1cgfo3b</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>This polish can legally drink alcohol</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpw8jnhikixc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1cgeoza</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Probably my cleanest job yet since I started painting last month!</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgeoza</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1cge72g</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Don’t sleep on Alchemy Lacquers!!!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cge72g</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1cgd34w</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Attempted some jade nails</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pb0lduhyzhxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1cgd1bx</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Golden Hour Palate Cleanser</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45yw0i2kzhxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1cgcw81</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>my new nail tech is amazing!!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8c5m20xgyhxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1cgcnd2</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Got my hands on La Luna!</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgcnd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1cgcb7p</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Moon Curse by Fancy Gloss</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgcb7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1cgc9tp</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Just got my some new polishes!❤️</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4g8jenhuthxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1cgbfvv</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>queen of rot</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgbfvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1cgb10c</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Vampy color for spring lol</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgb10c</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1cgaow0</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Fae or Foe</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79kr1txmihxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1cgamr7</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>A Most Destructive Melody</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgamr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1cgac3p</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Essie ballet slippers 🩰</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgac3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1cga27g</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Best magnets?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cga27g/best_magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1cg9pt6</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>What in Carnation 💐</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg9pt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1cg9jb2</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Anything is Popsicle from KBS and Holo Cherry from I Scream Nails are the perfect combo, summer strawberry vibes 🍓</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg9jb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1cg9dlb</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Do you ever feel guilty for not finishing your nail polishes?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cg9dlb/do_you_ever_feel_guilty_for_not_finishing_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1cg8ww1</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Actual Birthday Mani...</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fvfpqd96hxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1cg8uar</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Pre birthday man #7...</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/882wlufr5hxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1cg8qse</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>First attempt at any ‘art’</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg8qse</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1cg8idg</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>What is going on with my matte topcoats?</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cg8idg/what_is_going_on_with_my_matte_topcoats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1cg7fe6</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Lightning Strike 🌩</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg7fe6</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1cg7btd</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Blossom</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg7btd</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1cg73bt</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>ORLY - Sugarplum Soiree</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg73bt</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1cg6wcj</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Delivery day!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg6wcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1cg6s7t</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>LynB!</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg6s7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1cg6jl4</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Wandering - Ethereal Lacquer</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg6jl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1cg6era</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>I have some wild mixed feelings about this color! Also, anyone else experience shrinkage with Orly Sec n Dry?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg6era</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1cg6eg2</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Tried something new 🤓</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg6eg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1cg5z8h</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Dupe suggestions</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oez5ix5ilgxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1cg5yni</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Can I “fill” my dip manicure with regular polish?</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6e03vxdlgxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1cg5fyx</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>BKL Mirage</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg5fyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1cg2xg5</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>ILNP Unforgettable</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg2xg5</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1cg2a99</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>🔥😍❤️</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u43yuzc4vfxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1cg24aa</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Help - Nail tech didn’t completely remove my gel nails?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg24aa</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1cg1wrr</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>A guy looking for a gentle nail file</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cg1wrr/a_guy_looking_for_a_gentle_nail_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1cg1po6</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Careful, I Bite 🤍</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg1po6</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1cg170r</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Obsessed with the peekaboo shimmer in this jelly</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j1qnc8n7nfxc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1cg0ovm</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Dragonfly wings!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg0ovm</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1cg0lvr</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Women of a certain age/holo polishes</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cg0lvr/women_of_a_certain_ageholo_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1cg01c7</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Slimer/Shrek nails got me feeling like the Princess Of Prug 👑</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bp2dgilnefxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1cfzhvr</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Illudium Q-36 explosive space modulator</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfzhvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1cfyqzk</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Vanessa Molina Chewie (PPU Dec 2023) 🤎✨</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kiquro094fxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1cfyp1t</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Which nail shape would suit my hands?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfyp1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1cfxs33</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cfxs33</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1cfvg54</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Comparison of Clionadh Toxic Sludge and Whatcha Nightshade</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v861fq2t7exc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1cfvb47</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cfvb47/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1cgng2o</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>How do you rate my new work? 💕</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6wvbfikqkxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1cgmb7a</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>The absolute cutest custom press on nails! Love the stars &amp; gems!</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b55zvjhhckxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1cgjh1i</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Mis primeras Nailart</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgm2ba47ijxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1cggzac</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>I love clear glass like nails with minimal designs like these(set done by me)</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ll4uk4tovixc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1cgakk2</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Silver Chrome Anyone? IG@NailsbyTim6 </t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/od1r4gzshhxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1cga0gq</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Palate Cleanser Set 🤗 my builder sets arent hitting like I want to. I love a curved square, I’m wondering if I should taper it maybe?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dd97ycqxdhxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1cg9m7x</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Last minute nails to match my dress 💕</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg9m7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1cg8wmz</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>tropical spring duckies 🌺🤍</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85qob2k76hxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1cg7tqv</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>I have been experimenting with nail art!</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg7tqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1cg7tol</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>new nails :)</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg7tol</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1cg1qh9</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Gem Stickers! DIY</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cg1qh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1cfyimq</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time ever painting nails! Just wanted to share. More happy with this than anytime Ive ever spent money to get my nails done. </t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/veytt8wc2fxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed May  1 08:09:34 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_05.xlsx
+++ b/data/2024_05_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C460"/>
+  <dimension ref="A1:C617"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8253,6 +8253,2675 @@
         </is>
       </c>
     </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1chgcm0</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>My favourite Christmas set my nail tech did on me 🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chgcm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1chgauu</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Can I paint these and take nail polish back off without hurting the gel? My appointment is Monday and I have an event this weekend so I want to not have that gap. There's no extensions, it's gel on natural nails.</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o71lmf3xqrxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1chfzjl</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Nothing Sticks????</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1chfzjl/nothing_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1chfve0</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Favourite Shop to buy gel supplies</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1chfve0/favourite_shop_to_buy_gel_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1chf9co</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>How do y’all choose your design?</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chf9co</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1chf4js</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>What nail color/design would you do with this shirt? Can't be green and can't be too detailed.</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrctsupzcrxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1cgu28d</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>First nail set ever :)</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgu28d</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1cha9kk</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Nail damage after gel manicures</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cha9kk/nail_damage_after_gel_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1ch8je2</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Y2K inspired nails 🖤</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch8je2</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1ch7xe8</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Getting Gels after Heavy-Handed Buffing</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ch7xe8/getting_gels_after_heavyhanded_buffing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1ch7tn5</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>help!!!!!</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch7tn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1ch497v</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Doing the “tip” trend from TikTok, help me color match</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch497v</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1ch3hk3</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>What are some good airbrush color recommendations for gel x</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ch3hk3/what_are_some_good_airbrush_color_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1cgz2ez</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>my work/inspo from @qwjluna i loved the result!! what do you think?</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgz2ez</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1cgxq3u</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Why do my nails do this?</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85awxp10dnxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1cgx3wt</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Black gel with holographic top</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgx3wt</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1cgrvue</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Margin or error for new nail tech???</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgrvue/margin_or_error_for_new_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1cgrgqh</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>SHEIN nails, what’s the catch?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgrgqh/shein_nails_whats_the_catch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1cgqrcf</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Painting over gel?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgqrcf/painting_over_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1cgkv6c</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Tried solid nail glue for the first time and may never go back</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgkv6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1chdxr4</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>🩵 Matte Robin's Egg Blue (baby hand bonus)</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm7kbc9szqxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1chdn6h</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Press on Nail question</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1chdn6h/press_on_nail_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1chd6uw</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Sunflower and blue nails for sunnier days ahead</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t48od7tvrqxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1chd5i6</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Did my own nails🦋</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chd5i6</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1chd0i9</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>got them done over a week ago still love them</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to1dmpo1qqxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1chcp5s</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Almost 1.5 years in doing my own nails and the improvement I’ve made is amazing! Got this gold foil off Amazon…… 10/10</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eknx0oh4nqxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1chc1vv</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Is my nail ok? Are these cracks part of growing nails long or should I be doing something?</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zax80gqgqxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1cgofcz</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>blue nails :P</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgofcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1cha009</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>First time getting matching mani and pedi</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cha009</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1ch9xek</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>French Tip with White Pearls</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44qt2ersxpxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1ch9wan</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>very pink &amp; lovely. 💕</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wvwotrixpxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1ch9soj</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>fruit nails🍓🍋</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch9soj</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1ch9hjg</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Time for some purple [f28]</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gh0tvsk3upxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1ch9g6a</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Toes </t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iw42uw9stpxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1ch96zo</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>How long should I wait to put on new nails after I remove them?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ch96zo/how_long_should_i_wait_to_put_on_new_nails_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1ch8i7u</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Love This Design 🤩</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dguosz2tlpxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1ch8g1g</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t xml:space="preserve">diy nail oils? </t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ch8g1g/diy_nail_oils/</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1ch7zur</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Beginner nail tech 🤭</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch7zur</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1ch7aej</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Oldie Goldies</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch7aej</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1ch6v85</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Any advice for my nails</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ok1oxa6j8pxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1ch6hxx</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Boyfriend picked the colors, all I could think was a Joker theme</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch6hxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1ch66je</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>i cracked the tip of my acrylic!</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ch66je/i_cracked_the_tip_of_my_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1ch61tb</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Nails with appliqués!</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8abihpg72pxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1ch5u9o</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>red french on me by me❤️ is anyone else simply obsessed with french manicures????</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch5u9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1ch5sii</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>First time posting, how's my stamping?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbywsf190pxc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1ch5qn9</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My daughter got a new nail tech. </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcsedfmtzoxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1ch5ia8</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>First time with gel at home!</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch5ia8</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1ch5aot</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Gel polish over regular polish</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ch5aot/gel_polish_over_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1ch4y2u</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Gel galaxy nails</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdp58pi1uoxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1ch4i14</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Question about polishing over dip nails</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ch4i14/question_about_polishing_over_dip_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1ch3zd9</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>I've come a long, long way, and am going to keep it up! This is the difference 4 months of no biting &amp; regular maintenance has made to my natural nails! I'm loving my progress 💖</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch3zd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1ch3xug</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Fun design 🩵🖤</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch3xug</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1ch3kif</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Whoever voted round/almond…thank you :)</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch3kif</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1ch3bgm</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for alternative </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcfcubsbioxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1ch32mk</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>I love a good French tip</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rapx9xxhgoxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1ch30xh</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Anyone else have nails that curve up instead of down?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch30xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1ch2ec9</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>90s Vibes💖💅🏼🍟🍓</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch2ec9</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1ch29ky</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Milky mint with some glitter💚</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch29ky</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1ch245h</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Took off acrylics and tried a new shape</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3td4j7no9oxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1ch1esf</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Photos don’t do justice to the range of this shade</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch1esf</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1ch19w2</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>which nail shape suits me better? this is my first year ever getting my nails done so i’m still working things out!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch19w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1ch0r5q</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>💙🐳🤍🐟💙</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch0r5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1ch0in0</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Pinnacle Polish - North Cascades 🏔️</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch0in0</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1ch0ihl</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Loving this design! What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch0ihl</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1cgzzcy</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Wisteria Hysteria 💜</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgzzcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1cgzhh0</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>A new set of acrylics with matte top</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mthx34tcqnxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1cgyvra</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>First time using press on nails.. next time should I use smaller pieces?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgyvra</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1cgyjyr</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Orchid Nails St Pete</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgyjyr/orchid_nails_st_pete/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1cgydca</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>1st 💅🏼 of May</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xssuzli4inxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1cgy72e</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>What do you think? First time using a gel base and then a gel nail color.</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9qw9mpugnxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1cgy0mz</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling like my nails are finally pretty &amp; healthy </t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5o4kyqrkfnxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1cgxl95</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>First time doing French :) getting the lines straight and symmetrical is harder than it looks!</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgxl95</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1cgwy26</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>My favorite set from 2023</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upivf6y97nxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1cgwlpi</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>There’s no place like home vibes ❤️✨</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci4mnc0q4nxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1cgwh27</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>What am I doing wrong</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s00c7xjs3nxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1cgw8au</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>It's not perfect but I only qualified in January so I'm working on it 🥰</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4be3d7gz1nxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1cgw6w8</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgw6w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1cgw0wc</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Third time ever applying press ons, I think I’m getting better!! So in love with these ones! CCW!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgw0wc</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1cgvqip</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Grey &amp; Gold 🩶💛</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ocdf14bymxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1cgv93y</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>I need some help</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oc4qphloumxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1cgv5le</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>🐆 nails</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5l3bbwytmxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1cguy3p</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>My honeymoon nails! These ones definitely took some patience</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ik52y9ismxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1cguvhn</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>How is my crystal placement?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cguvhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1cgun8f</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Royal elven set</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgun8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1cgtzwi</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mixed Media Mauve by Finger Paints </t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3qx43w8lmxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1cgsqpw</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Second time I've accidentally twinned with my drink!</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgsqpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1cgsc5j</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>This black kitty sticker set is one of my favorites! 🐈‍⬛💖</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgsc5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1cgsbv4</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>[DIY] these decal nails!</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxnyea0u7mxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1cgs81t</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried to do ombre with an ombre brush. Any tips to make the gradient more smooth? </t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcn5fjj07mxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1cgqzpv</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>🩵 My April Manicure 🤍</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0uh1tekuvlxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1cgqts3</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Neon</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgqts3</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1cgqtgp</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Holo is the way ✨️</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9crcsmv4ulxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1cgqfsd</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Noob question about nail glue 🙋🏻‍♀️🤷🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cgqfsd/noob_question_about_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1cgqdpl</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Quite probably my favourite gel overlay set I've ever done</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgqdpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1cgoqpf</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>First time sharing here🥰</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgoqpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1cgomjk</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Sometimes I go back to nude</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjuekdwe5lxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1cgo17a</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Honest opinions</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgo17a</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1cgnrp3</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Burlesque!</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2rkks6iukxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1chfekt</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Some manis from Feb/March that I kept forgetting to post (including a Boolba skittle!) 🌱</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chfekt</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1chepnt</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Obsessed with Portrait of an Introvert</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chepnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1chd61r</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>solid colors</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1chd61r/solid_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1chd4jn</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Wheezing and coughing days after accidentally in halo be nail polish fumes?? Should I be worried?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1chd4jn/wheezing_and_coughing_days_after_accidentally_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1chcg80</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>“Oxfords not Brogues”</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chcg80</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1chaxpf</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Cactus Jelly 🌵✨</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chaxpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1chapo7</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Got inspired🥰Which hand do you prefer?🌚🩸🎂</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chapo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1ch9uup</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Beaux Reves Polishes</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ch9uup/beaux_reves_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1ch9sx2</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>very pink &amp; lovely. 💕</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbswiswpwpxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1ch972r</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Mooncat Disappointment</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch972r</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1ch90tq</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do my nails look  weird? </t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrjg8rk6qpxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1ch7mw8</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>How to achieve this effect?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtpwl9kvepxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1ch7hqa</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Sally Hansen: in the shade Augmented Red-ality.</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dn5q6euodpxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1ch77c4</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Honoring Grandma</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch77c4</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1ch6khq</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>We are the weirdos</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch6khq</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1ch663f</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>BKL — a warm welcome</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch663f</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1ch4uqt</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>When your nails match your car 🥵</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch4uqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1ch4tyb</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>All polished up and no where to go!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch4tyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1ch4mke</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>I took "claws" way too literally 😝💅</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1plxavbsroxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1ch4f8i</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Let's Talk About Neons</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ch4f8i/lets_talk_about_neons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1ch49hp</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>All of March and April’s sparkles and glows ✨</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch49hp</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1ch3rxs</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>My first thermal - Flaming Zombie by LynB Designs!</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch3rxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1ch38xf</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>blurple with gold? groundbreaking</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q020zl3thoxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1ch1v2p</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>shimmer skittle ✨</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch1v2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1ch1mvs</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>My nails a year ago vs today (+ more pics of my current mani)</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch1mvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1ch1c2x</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Iridescent Cellophane</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch1c2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1ch1c14</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>RIP nail</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gl1ikgs3oxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1cgzv84</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>First time trying gradient on my nails. Any help to prevent the muddiness of the center color?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74ykh4h4tnxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1ch146k</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Spring Flowers 🌼</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch146k</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1ch0oyb</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Springy</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch0oyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1ch0j88</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Help switching back to normal polish?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ch0j88/help_switching_back_to_normal_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1ch0ha6</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Pinnacle Polish - North Cascades 🏔️</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch0ha6</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1ch06lx</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>April manis!</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ch06lx</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1ch000o</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Velour </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1dul7v3unxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1cgyotr</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>It’s one banana, Michael!</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vkgs4bgknxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1cgxwor</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Dream Within a Dream &amp; Mood Ring (Cirque Colors)</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgxwor</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1cgwu22</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>It’s like funfetti cupcakes on my fingertips 🧁</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvld5xjf6nxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1cgwbca</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Journey to stop biting my nails, a success story.</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cj1ocfm2nxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1cgvrt1</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Grey &amp; Gold 🩶💛</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bax9gvkkymxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1cgux4e</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Flashing Lights ✨</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgux4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1cgutjx</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Something is blooming- better take a picture of my nails in front of it!</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dewe36qirmxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1cgute0</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>First press-ons made for Spring!</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgute0</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1cgtpbj</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Love when 2 of my hobbies meet 🖤</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgtpbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1cgtcn0</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>BKL Lemon siblings…</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cgtcn0/bkl_lemon_siblings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1cgsnhc</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>That GLOW</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgsnhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1cgreq7</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Feeling the holo✨️</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wj2vdtpozlxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1cgqtxk</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Cuticula understood the assignment 🧡💙</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4pm7hm9ulxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1cgqlhg</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>A England Lachrymae</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgqlhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1cgqg08</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>It’s hard to believe that all of these are the same polish</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgqg08</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1ch9v5y</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Used paint instead of polish </t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dz0bjvz8xpxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1ch8mev</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Maggie Simpson</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbanf6rsmpxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1ch3c0c</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>sparkly french tip</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6d8m828gioxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1ch22ne</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>My new work ❤️</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugbrz1uc9oxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1ch1xur</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Spy x family set took 4 hours😪</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3a8h04d8oxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1ch1a2u</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Tried ombre and matte... how do you clean up edges / cuticles?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0kvndee3oxc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1cgxstu</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>first nail set</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uo5mixkkdnxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1cgum5e</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Royal elven set</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgum5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1cgpql4</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Vacation nails by me</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qk6j81mlilxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1cgohfx</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>My first character nails any tips? RICO NASTY✨✨✨</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cgohfx</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu May  2 08:08:38 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_05.xlsx
+++ b/data/2024_05_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C617"/>
+  <dimension ref="A1:C749"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10922,6 +10922,2250 @@
         </is>
       </c>
     </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1cia5sp</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Halfway to Halloween but still springtime!</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhl3gej80zxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1ci9qmc</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Cozy nails 🤗 I did them with Gelish temperature change nail polish, cute embossed stickers that I got on Amazon, and a top coat ☕️🧁</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci9qmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1ci8gj7</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Real red nails</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7qhtu80gyxc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1ci7tjv</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Mermaid set. What we think about it? 🧜🏼‍♀️🩷🐚</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hz0kqfby8yxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1ci7nb6</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Please help</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ci7nb6/please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1ci6qr5</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Nails grow in different shapes?</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p63muwnoxxxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1ci6kf5</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Beach Nails</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci6kf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1ci6bxr</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Need help with nails</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uboeerftxxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1ci5skx</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Recent nailsets that I've made</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci5skx</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1ci5os3</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Are back to back builder gel manicures safe?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ci5os3/are_back_to_back_builder_gel_manicures_safe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1ci5n5k</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Korean gel nails</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci5n5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1ci5g0m</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Taking back my nails</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ci5g0m/taking_back_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1ci51lk</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Aquarium light !</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khega5b8hxxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1chxyi7</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Went and got my nails done yesterday, what I got vs. what I asked for. Original inspo pic from @nailedby.tati on IG</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chxyi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1ci4akh</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Slay or nail for my first time?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci4akh</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1ci3yan</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Best nail glue for press on nails</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ci3yan/best_nail_glue_for_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1ci3v3l</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Plain but cute 😁</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci3v3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1ci3bf5</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>First time applying rubber gel 😅 what do you think?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5l2irepr1xxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1ci359e</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Daughters color choices💕💜💅</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2ut87jb0xxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1ci2phk</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>I did my first gradient today and I’m so proud of how it turned out!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci2phk</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1ci2alh</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>recommendations for products/homemade recipes to strengthen my nails?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgecbkj3twxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1ci1tuw</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Night Skies</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci1tuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1ci1a10</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Getting this pink always reminds me of my beautiful momma 💗</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2mfnrspkwxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1ci188h</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Lost a nail somewhere ....can't find it...was complaining..my 10 yr old son said he had a solution 🤭🤭🤣🤣🤣🤣🤣😅😅😅</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epu6q7ibkwxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1ci17nb</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>How should I shape/file my nails?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci17nb</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1ci12tp</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Flores de Mayo Nails</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci12tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1ci0nr6</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Went for something simple</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci0nr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1ci06li</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>All white</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4o6lw92cwxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1ci01i1</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>i 🤎 press ons ✨</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci01i1</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1chzitw</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>When I'm forced to do extensions</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chzitw</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1chz1zn</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Nail shape advice</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chz1zn</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1chyx5a</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Esculpidas french técnica reversa</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chyx5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1chyg8g</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>some of my favorite nail sets ive had</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chyg8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1chxzrm</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some spikes for this weeks set </t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrke9un6wvxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1chxf0j</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>🌷🥰</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aehmxus0svxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1chwzoe</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Base coats?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1chwzoe/base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1chwhsp</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Spring 🌸💙</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tycg158alvxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1chwdhv</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Fresh gel overlay</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2so02g3fkvxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1chwan6</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>made the cutest press on nails for my client🦆🩵🐸</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chwan6</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1chwaam</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Had my first Russian manicure and I’m never going back💅🏻</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chwaam</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1chw3gn</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>used to be a prominent nail biter, these are my current nails :)</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chw3gn</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1chvzca</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Cute and simple 🤍</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5hop7cfhvxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1chvu8s</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>My amazing nail artist brings out my inner pastel goth (BIAB)</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n17kjbgegvxc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1chvu6h</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Just noticed that my new mani is the same color as this guava juice I made 🍈</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w75tolzdgvxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1chvk88</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>3 week change up</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n42a5uvfevxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1chv8og</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Cuticle/ nail question!</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gq1tmi21cvxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1chuv2w</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Which shape suits me best??</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chuv2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1chtgsu</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Why does my nail polish never last??</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1chtgsu/why_does_my_nail_polish_never_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1cht76v</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Get your inspo and go</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cht76v</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1chqp1x</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hard gel and acetone (Removal/Soak Off) Let's discuss the science behind it and terminology! </t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1chqp1x/hard_gel_and_acetone_removalsoak_off_lets_discuss/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1chqe7i</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>How do you prevent press-ons from lifting at the nailbed?</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jndavl1duxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1chm8ka</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>How do I fix my nail</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chm8ka</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1chief3</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set for the summer :) </t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyncll6tgsxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1chgxz2</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Why does my nail keep breaking so far down</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ejm8ho5zrxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1chevp3</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>sally hansen miracle gel application help</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1chevp3/sally_hansen_miracle_gel_application_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1chut2p</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Which nail shape fits my hand better?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knfakz2t8vxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1chuimv</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Le mini macaron </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1chuimv/le_mini_macaron/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1chudqg</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Am I tripping?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlctwi4p5vxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1chubq0</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>May set.</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chubq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1chtu56</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Trying to grow my nails but I wear gloves all the time..</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chtu56</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1chtnq1</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>First post on here!</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chtnq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1chsi23</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>I'm very bad at painting my nails, but I love seeing them black</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chsi23</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1chselr</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Colorblock nails</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnujvbqrruxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1chrwvu</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>So happy with the result💚</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mly0d64ouxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1chrqka</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cheap nail polish vs. expensive </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1chrqka/cheap_nail_polish_vs_expensive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1chrqdp</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Update: is this better?</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chrqdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1chrj0d</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Birthday nails!!</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q94vkojbluxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1chrf4n</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails update! </t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tr7tlffjkuxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1chr8kc</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Can you buy Dazzle Dry in stores?</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1chr8kc/can_you_buy_dazzle_dry_in_stores/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1chqggk</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Cowboys &amp; Sunsets</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrfukogiduxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1chpllv</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Pretty proud of these berries</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.imgur.com/a/I13oqIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1chomnc</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Ive been getting claws for years. Finding my way back to Chrome.</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chomnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1cholea</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Proposal nails (but I didn’t know it!)</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cholea</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1choki3</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">can i get a fill if my natural nails are as long as my acrylics? </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1choki3/can_i_get_a_fill_if_my_natural_nails_are_as_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1chogzq</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Took me an hour, really happy with the results 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chogzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1chnz8a</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Pink chrome🔮🤩</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chnz8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1chnm0q</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>The most gorgeous set I've ever had 🖤🖤</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xp5gxvzbstxc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1chnbz4</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>My nails are finally growing!</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw3aw6r3qtxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1chm438</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>felt like this acrylic set was pretty good for only $45🤩</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chm438</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1chluqd</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Aura nails ✨</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k48wzalfetxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1chll1m</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Is there anything a nail tech can do to my broken middle finger to make it even, that isn’t acrylic?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9im6b19ctxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1chljcy</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Ohora gel wraps in “Blush”</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chljcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1ci7qzn</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Mooncat Beowulf 🐺🌿</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6n0rt0468yxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1ci5kyt</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>This sub is my huge inspiration for keeping my nails painted so they grow, so I thought I’d show today’s paint job :)</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci5kyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1ci4zul</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>The Sun Will Rise and Warm You Today</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xaufd19rgxxc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1ci2pc0</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>"It was alive and glowing and vibrant...</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci2pc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1ci2ip8</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>“I Thought the World of You”</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci2ip8</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1ci1ptw</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Fallen Angels</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci1ptw</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1ci1cuw</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>this month’s nails: april 🌷</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci1cuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1ci0yr1</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Vacation Nails</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bawdc778iwxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1chzv9w</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>My new favorite red for the summer. ❤️</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chzv9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1chz3og</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Paint the town red 😍❤️</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qid3kt04wxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1chysd7</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>The Gel Bottle BIAB High Gloss Top Coat getting dull after about a week</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1chysd7/the_gel_bottle_biab_high_gloss_top_coat_getting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1chyi84</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>They really missed the boat</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9uutv6mtzvxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1chyem4</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Queen of Rot is my true love</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chyem4</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1chyc9t</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>April manis!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chyc9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1chxnuj</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Toothless the Dragon inspired</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chxnuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1chxjoz</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>A little something different for me</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chxjoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1chx6zu</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Spring skittle 🌸</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chx6zu</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1chwx0h</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>What I wore in April</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chwx0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1chvulo</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>little fox 🦊🧡</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chvulo</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1chv9jm</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>It's a gloomy spring day. A moody green seemed fitting.</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chv9jm</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1chu2yh</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Ice Cream Sea 🍦</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chu2yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1chtxkw</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Peeling nails</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1chtxkw/peeling_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1chteoe</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Gravity, Hold Me Back</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chteoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1cht39e</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Whenever I’m bored and the mani is still good, I slap on a matte topcoat</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhsjso6kwuxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1chszn7</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>What color,  or what's similar??</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34ql9sbvvuxc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1chrdg2</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>ILNP - Bluebell</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ndjwqti6kuxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1chr19y</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Am I doing GG Top Coat wrong?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh4jzlsqhuxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1chqq9d</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>First time doing my sister's nails</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chqq9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1chqnah</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>FAVORITE Linear Holos</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1chqnah/favorite_linear_holos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1chpzz0</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>why do my nail layers split like this while filing?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlshv756auxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1chpwcg</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Indecisive blue mani</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chpwcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1cho7uw</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Oh, me? Just wearing my favourite ILNP ever 🤩💜</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vix0axdzwtxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1chnau1</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Does it give dark fairy or Halloween? 🧚‍♂️🎃</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdxgujdwptxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1chn1c1</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Layered with touch of velvet</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1tszyznwntxc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1chmcgx</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Rain Shower and Pitter Patter on rainy days (w/ my bestie making an appearance in the background)</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chmcgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1chm277</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Looking for a swatch comparison: Holo Taco’s Never Tide Down vs. Mooncat’s Maelstrom</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1chm277/looking_for_a_swatch_comparison_holo_tacos_never/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1chls0u</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>When layering goes right ❤️</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ilyxizsdtxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1chl1mr</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Toucha Touch Me</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chl1mr</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1chijwa</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Have you ever given up on a polish you wanted to love?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chijwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1chidcp</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1chidcp/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1chicxf</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1chicxf/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1chhv42</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I stain my gel manicure? </t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1chhv42/can_i_stain_my_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1ci7d75</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Bday nails 💕✨</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci7d75</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1ci6nda</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Nail pic dump 💕</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci6nda</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1ci6lit</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Beach Nails</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ci6lit</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1ci0avv</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>🦋🦋🦋</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q24nctyzcwxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1chx2bh</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blossom power puff girls tutorial </t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3uybasfhpvxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1chwb6z</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>made the cutest press on nails for my client🦆🩵🐸</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chwb6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1cht7u8</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Birthday set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98b1j0ygxuxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1chqc8n</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Life</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1chqc8n</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri May  3 08:08:36 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_05.xlsx
+++ b/data/2024_05_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C749"/>
+  <dimension ref="A1:C915"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13166,6 +13166,2828 @@
         </is>
       </c>
     </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1cj37j9</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Builder gel, how do these look to you?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zy0n3xgp46yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1cj26n9</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Ombre Summer Nails ☀️ still learning but second ombre went waaay better</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj26n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1cj1m7y</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>❤️💛</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj1m7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1cj1jyt</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Did gel color for the first time</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ccr17nak5yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1cj0yd0</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>One of the most beautiful manicure I’ve had.</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj0yd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1cj0xd4</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>NAILS!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj0xd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1cj0roh</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>I’m a press on girl for life tbh</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj0roh</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1cj0h45</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>I said no 😍</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chf4fsv385yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1cizwuk</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Is it necessary to cut natural nails before press ons application?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cizwuk/is_it_necessary_to_cut_natural_nails_before_press/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1cizs1z</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>In love</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cizs1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1cizahp</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do you like my nails? 😍 </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cizahp</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1ciz6zx</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>guys which looks better with my new tan pink or purple</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciz6zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1ciz3c7</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>New Here! Check out my animal print nails!!</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciz3c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1ciz1lh</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>simple but i like it!</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciz1lh</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1ciyv3x</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting completely free redo or refund - thoughts? </t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsw1wm70s4yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1ciyqxj</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>3D flower 💗</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciyqxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1ciyqf4</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>I love them</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpuu4tgpq4yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1ciyoqn</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>natural nails !</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciyoqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1cixq0u</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Nail shapes</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnf82wb7h4yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1cixeof</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Tips for getting nail gems to stay on longer</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k58l1k8be4yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1cimhyn</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Is there someone / a way I can pay someone to design nail art or moodboards I ask for at a local salon? I have some ideas for inspiration, but not how they'll apply to a do-able nail art.</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cimhyn/is_there_someone_a_way_i_can_pay_someone_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1cisu2n</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>clueless guy needs help</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cisu2n/clueless_guy_needs_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1cifpqn</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Pink obsession😍💖inspired by my internet bestie u/Amioix</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cifpqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1cix03v</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Too much?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hirl1ctpa4yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1ciwxk5</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Nail techs in Colorado</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ciwxk5/nail_techs_in_colorado/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1ciwuqr</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Broken nail</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ciwuqr/broken_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1ciwpbz</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Russian manicure</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgpk4f3y74yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1ciwmb5</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Spring nails💛</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cs929cx674yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1ciweiw</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>My last 3 nail sets, love my nail tech</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciweiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1ciwdkg</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Impulsively got blue tips last week! Am in love!!</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggmiaa7154yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1ciwbjb</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Weather is good, nails are good, all is good.</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciwbjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1civrji</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>I just love almond nails! ❤️</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1civrji</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1civpeq</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Did I do something wrong?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1civpeq/did_i_do_something_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1civ8fz</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8e6n9csu3yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1cius6s</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Off to get married this weekend! My bridal nails.</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulpqkoovq3yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1ciur40</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>I love this color</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frxcjiimq3yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1ciuaeq</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Read about Russian manicure on here so saw what that was about today. Seems ok?</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oj0zjy5nm3yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1ciu5bv</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>How much should I have paid for these?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciu5bv</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1citt38</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Builder gel is my new favorite 🌷</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1citt38</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1citqcc</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Loving this cherry set</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1citqcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1citodw</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Violet Galaxy Nail</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/abt2sz8nh3yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1citnp9</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vertical rainbow ombre! </t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0dfytzqfh3yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1cit5q4</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Is it safe to let my gel nails grow out instead of removing the gel? If so, can I file to shorten it?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cit5q4/is_it_safe_to_let_my_gel_nails_grow_out_instead/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1ciseg6</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>My second time ever doing my nails as a 21 year old typically masculine guy</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciseg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1cis8u9</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>nails</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cis8u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1cis1ph</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>former nail biter! here's my progress &lt;3</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cis1ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1cirfbw</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Curing Gel Nails</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cirfbw/curing_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1cir9mw</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Why do I hate them</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cir9mw</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1cir2qf</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What method is recommend for beginners? </t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cir2qf/what_method_is_recommend_for_beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1ciqxx1</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>$100 gel Mani and Pedi. Mobile nail tech</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciqxx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1ciqs68</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>fresh set!!!</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xg0hun9v2yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1ciqmrt</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Growing my nails for the first time in my life. Any tips, tricks or advice for me? Would be greatly appreciated </t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ciqmrt/growing_my_nails_for_the_first_time_in_my_life/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1cipmue</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>some little blueberries for my first time posting here!</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cipmue</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1ciogbo</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Do I do too much house work for gell nails?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ciogbo/do_i_do_too_much_house_work_for_gell_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1cio5yj</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Equivalent of Cabernet with Bae miracle gel?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cio5yj/equivalent_of_cabernet_with_bae_miracle_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1cinmdk</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Same Garden of Evil, less face</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cinmdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1cingkn</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nail artist - Canada </t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cingkn/press_on_nail_artist_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1cine9b</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Aura Nails with Blooming Gel - Help!</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cine9b/aura_nails_with_blooming_gel_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1cindj2</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>New nails 😺</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cindj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1cimqch</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Snake nails idea 💫✨🫶🏻</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4r759d222yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1cilq7z</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Babymoon Nails 🌝</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34yujqdsu1yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1cil8l0</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>What does this review say about the salon</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hutk5653r1yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1cikoh5</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Can I file to reshape dipped nails?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cikoh5/can_i_file_to_reshape_dipped_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1cikf9r</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Matte Blue 💙</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sflybft4l1yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1cijn5d</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Best strengthening products for natural nails?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.opi.com/products/treatments-strengtheners-nail-envy-all-night-strong-nail-strengthener</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1cijlmk</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Fix?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scjzf5o4f1yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1ciipgx</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>New favourite 🤍</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45sn1umt81yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1ciioc3</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Where can I find these?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciioc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1ciik3c</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Just started experimenting with gel polish! second set i’ve done with it 💕💫🌺</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xbfjbbr71yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1ciide1</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is BIAB or BioGel better for your nails? </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ciide1/is_biab_or_biogel_better_for_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1ciia7p</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>My favorite nails I have ever done 🥺</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2w0nmnfs51yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1cii18i</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did a friend's nails today! </t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkwhl2ay31yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1cigxvs</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Thoughts on my current nail shape</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cigxvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1cigwun</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My mermaid nails </t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dlx21jcbv0yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1cigtym</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - Ghosts in Ectoplasmic Color 👻</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cigtym</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1cigrjr</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>I hate how thick acrylics and gel-x are. Alternatives?</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cigrjr/i_hate_how_thick_acrylics_and_gelx_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1cigkpc</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>I go to Hawaii tomorrow so I did these 😁🌊⛱️🌺</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ez64ag1ys0yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1cigcp7</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Russian manicures are the way to go</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cigcp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1cifzss</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Is it May yet? Indy 500 nails! 🏁🏎️</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cifzss</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1cifpxr</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Flormar Full Color in Squashed Raspberry</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cifpxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1ciexkl</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Just create a new one for high comfort, do you like it?</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5lnpoevf0yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1ciew3f</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Rubber gel base and clear top coat coming off at restaurant job after a couple of days. Is hard builder or polygel better for short bitten nails not to add length, but to last?</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ciew3f/rubber_gel_base_and_clear_top_coat_coming_off_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1ciesge</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Help - SO wants me to pick their nails but I don't know terms</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ciesge/help_so_wants_me_to_pick_their_nails_but_i_dont/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1cidtbf</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Appropriate med student nails</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjrwm7vt50yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1cid60a</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Nail set advice !</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cid60a</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1cicnm3</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>First time trying French with dip! 🎀</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cicnm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1cicl8r</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Made a post about not being able to choose a color. I chose a color today</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbavxtdxtzxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1ciblu2</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Spring set 🌸</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bi279u0vizxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1ciavdb</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Ocean mood😃</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciavdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1ciaull</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How often should I apply strengthener to my bitten down weak nails? </t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ciaull/how_often_should_i_apply_strengthener_to_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1ciarrg</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Nail shape</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61cenhy58zxc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1ciabur</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>how do y’all stop from accidentally picking your fake nails off?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ciabur/how_do_yall_stop_from_accidentally_picking_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1cizpcd</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Press on+cuticles</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kwrkbo405yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1ciz0pc</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>You never go full fecal sample</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciz0pc</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1ciysd6</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Dating this vintage polish</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciysd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1ciybyk</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>ILNP Deep Space</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3mdqlfrum4yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1cixiur</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>LynB - Zoisite</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cixiur</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1cix5b2</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>HEADS UP 🌕 Mooncat sale, finally</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jb36pg1c4yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1civx3v</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Matching my mani and pedi</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jx1msom014yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1civnyi</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Looking for recommendations!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzl9dzqpy3yc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1civccg</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Springtime bling! </t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id029kwqv3yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1ciuk6o</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Naydra is STUNNING</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/96cm9mxxo3yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1ciu50w</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers and Krisable Designs - April PPU</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciu50w</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1citw7q</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>How dare you</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37yukn1fj3yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1cits4w</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cits4w/what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1citkwz</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Potion polish across time dupe?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1citkwz/potion_polish_across_time_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1citjep</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>My first PPU and oh My!</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1citjep</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1cit8rq</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>One of my all time faves 🪴</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5idxinz5e3yc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1cit5ey</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Eek love Careful I Bite but it came out sooo bubbly!</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cit5ey</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1cisv26</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I saw someone take a pic of purple glitter in front of lavender, so I took a pic of purple glitter in front of lavender. </t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80cu25r1b3yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1cishzi</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>April manis + nail growth progress</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cishzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1cisclo</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>BKL Morocco but make it scientific!!! also new nail shape?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cisclo</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1cis0ey</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Did some spring nails recently 🌻</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gntoul1k43yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1cirhj7</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>New nail girly and I need help</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cirhj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1cirf9j</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Kbshimmer's Pool Shark</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cirf9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1cir2vg</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I call this piece "Heartbreak at the Gym" </t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14n7h8shx2yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1ciqypi</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Thinking of a good title.. 🐈🐾💜</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqx0dhmmw2yc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1cipkf5</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Wildflowers Skittle</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ucgebwcm2yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1cipfut</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>🔵 Now you're thinking with Portals 🟠</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cipfut</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1cip7et</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Help seeking drugstore/Sally Beauty-accessible dupe for Holo Taco Pink Smoothing Base</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g106m7wvj2yc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1ciotjw</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Candy nails and Topcoat question.</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciotjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1ciosmo</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>This might be the prettiest turquoise I’ve ever seen ✨ Polishes Used: Cirque Colors (Shade: Elixir of Everlasting Life) | Essie (Shade: Good to Go Top Coat)</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciosmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1cioonu</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>I saw someone on here do orange and pink nails so I did orange and pink nails 🍊🌸 Polishes Used: Pinkie and Pointer Fingers, Zoya (Shade: Rica) | Ring and Middle Fingers, Zoya (Shade: Matilda) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cioonu</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1ciojvo</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>This color is so fun and summery! Polishes Used: What Addiction? (Shade: Kelp Forest) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciojvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1cioghl</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>I don’t do cremes often but this turned out beautiful 🍓 Polishes Used: Orosa (Shade: Fig) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cioghl</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1ciocuk</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Pistachio Please</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciocuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1cio7dn</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Another indie dupe for Mooncat!</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/taey9otrc2yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1cinhff</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Moody Skittle</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cinhff</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1cingp9</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Looking for a dupe. It is Gelcare Rose Water.</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93c4i3je72yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1cinaot</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>I'm Blue (Da Ba Dee)</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrudc4p462yc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1cin8a2</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Mermaid mani 💅</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxh1opmm52yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1cim7ua</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Comparison of green linear holos</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cim7ua</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1cilpvt</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Does anyone have swatches of both Mooncat’s Forbidden Cove &amp; ILNP’s Hex??</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cilpvt/does_anyone_have_swatches_of_both_mooncats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1cikhq8</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are these too similar? </t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cikhq8/are_these_too_similar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1cikckf</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Russian manicure? </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cikckf/russian_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1cik7vy</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Horseshoe Magnet🧲✨</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/retqiyjnj1yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1cijw6n</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>I think this is my all time favourite polish</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cijw6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1cijof1</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Oh she glows</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zh05x87of1yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1ciivim</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Iridescent Coquette</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciivim</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1ciiipg</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why is my gel topcoat turning opaque? Recommendations? </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jd1p89hh71yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1ciieif</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Recent fun find, got me thinking about toppers</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciieif</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1cii3ea</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>🦀</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cii3ea</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1cihrr4</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>How do I make my capped edges last longer than an hour?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cihrr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1cih4lc</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Final fantasy</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agdx31b7x0yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1cigxpk</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - Ghosts in Ectoplasmic Color 👻</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cigxpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1cigptn</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>I finally found a magnet setup that works well for me</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zqc469zst0yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1cifr2g</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A overcast day means multichrome 🔮KBShimmer 'No Illusions' </t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovfz11mnm0yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1cifovz</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Can I used silk wraps under full cover tips/ Gel-X extensions?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cifovz/can_i_used_silk_wraps_under_full_cover_tips_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ciez4u</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Bluebell by ILNP is stunning 😍</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pivh7mfg0yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1cie5l4</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>⚡️☢️FALLOUT☢️⚡️</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cie5l4</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1cic7ww</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is a review justified </t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cic7ww/is_a_review_justified/</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1cibxy0</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Eco friendly swatching sticks?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cibxy0/eco_friendly_swatching_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1ciai9p</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>🥹 it's so beautiful</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciai9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1cj21ph</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>too my cherry set off a week early because i broke the pinky</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj21ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1cizi7p</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Sailor Moon nails (with chrome)</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxnt6vu6y4yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ciyimm</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art (last photo is what I was aiming for)</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ciyimm</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1ciyf7r</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Super mario nails </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/boyh95won4yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1cixpho</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Tomorrow this beauties that accompanied me on my birthday have service 💅🏼💗🤍</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cixpho</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ciwn78</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Fun Chrome Set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftxl8lle74yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1civysr</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>One of my fav set I’ve ever done</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b5e36hvf14yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1cit6uo</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this set i made, do you like it? </t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gefog9rpd3yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1cit1ml</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Moth Season DIY</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cit1ml</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ciq5oa</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>First time doing the 3D acrylic flower 😊🌸</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7p0fjxzlq2yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1cijiud</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>in love💖</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yonaqnf8e1yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1cihf80</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>👏Advice needed. I always struggle with background with character nails. What can I do to the background to improve the design or is simple better? 🤔</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cihf80</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1cicwxy</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Need some advices to start again, please</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1cicwxy/need_some_advices_to_start_again_please/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat May  4 08:07:30 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_05.xlsx
+++ b/data/2024_05_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C915"/>
+  <dimension ref="A1:C1064"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15988,6 +15988,2539 @@
         </is>
       </c>
     </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1cjsx7y</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>What nail shape should I get?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4cw37n3cicyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1cjuf6h</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Impress press ons</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjuf6h</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1cjtvx2</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>fresh set 🌸</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aulj93oktcyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1cjt1d3</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Loved doing my own nails so much I'm now enrolled in the nail tech program at Brown Aveda! It has been very fun learning everything there is to know about nails</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjt1d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1cjsm6v</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>fun prom nails</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjsm6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1cjsc38</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>French Chrome ⬜✨</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjsc38</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1cjqt9a</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Chainsaw Man Themed Nails 🖤</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6t2qmt64wbyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1cjqonp</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Using nail art brushes </t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cjqonp/using_nail_art_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1cjp46x</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>How do I use this? What's bonder? Also, What colors am I missing to have a perfect collection?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjp46x</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1cjo7rn</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>How do I tell the person who painted my nails they did a bad job ?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cjo7rn/how_do_i_tell_the_person_who_painted_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1cjla0z</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>What are methods or aftercare that will help me keep glue on nails longer? I prep the nail bed, do foundation, top coat, file the TC for roughness, sand a bit of roughness into the fake nail, and then a drop of glue... Often fall off starting 1-2 days after applying.</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3vvt3abhayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1cjkrwo</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>help me pick a shape please</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjkrwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1cjetpf</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Product Rec for long, healthy natural nails? Gel/base? </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cjetpf/product_rec_for_long_healthy_natural_nails_gelbase/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1cjd7ms</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Gel X and moisture, tips/products?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cjd7ms/gel_x_and_moisture_tipsproducts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1cjbg50</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>My favorite set so far!</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjbg50</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1cjay3x</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Acrylic for wedding?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cjay3x/acrylic_for_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1cjgyl0</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>The Claawww</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjgyl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1cjqodt</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>I came to change it to something brighter, I'll show you the result later</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2cneltqubyc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1cjqihh</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Practicing my nail art skills</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjqihh</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1cjqb6d</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>A little sad today but what y’all think?</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivzo8la7rbyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1cjq9my</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Neon tips</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjq9my</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1cjq0d0</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Manual labour manicure.</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gttcztgbobyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1cjpbtq</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Nude with silver chrome!</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjpbtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1cjoryu</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Done on me by me!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhaqzhdccbyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1cjomob</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t xml:space="preserve">beep beep </t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1q4k1oxabyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1cjo9p9</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>My second time getting acrylics, why don’t I do this all the time???</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cra8kocg7byc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1cjo95o</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>guy here, constructive criticism on my schnails?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yjfwfpb7byc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1cjo8je</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Not a glitter fan, until now✨</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wk54chw57byc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1cjnqpk</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Got my nails done for the derby!</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2ikcmil2byc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1cjnl1g</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Russian mani- first time</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjnl1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1cjnasg</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Behold! My 180⁰ nail! </t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kguq9umnyayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1cjn6rc</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I've always been drawn to Fall colors.. </t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nak5oxjnxayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1cjn6e6</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Acrylic with gel + pigment</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjn6e6</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1cjn4nv</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>They are a bit blurry</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjn4nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1cjn2cn</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Did this set on my mom for Mother’s Day 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gqy0avkwayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1cjn1ru</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Have been dying to trade in the claws for a nice short set 🎀 (still love my long nails just needed a break lol) </t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pouu5kfwayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1cjn0y8</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New design </t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqcxmgd8wayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1cjmjyt</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>So much love for this polish 😍</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjmjyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1cjluj9</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Silver nails with gems</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjluj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1cjkopr</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Sunset nails using pigment powders 🧡</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zeccepdicayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1cjkepg</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>I am in love with this blue</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjkepg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1cjkbos</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Any other gamers get your WASDs shorter?</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g999665q9ayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1cjkb3u</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Springs here and so are the bright nails</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjkb3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1cjinzl</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t xml:space="preserve">keeping it simple </t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9xykw47x9yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1cjihrk</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Just a simple transgender flag to celebrate my degree and all I've been through</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/873kiraiv9yc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1cjhwx3</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>CVS nail tops and gel overlay?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cjhwx3/cvs_nail_tops_and_gel_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1cjgz8h</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Delicate design to change the French 🤗</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjgz8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1cjgr28</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>A spooky way for me to stop biting my nails lol</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tz4ihrevf9yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1cjgc9i</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>biab + gel polish</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjgc9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1cjg7mu</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Never Know What Design To Get</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etn9jn5rb9yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1cjf016</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>did some little strawberries for my mom so we could match</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjf016</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1cjerw0</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still learning to do my own 🥰 </t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4yd5eqz09yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1cjeoz1</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>DIY press on nails + classic red</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjeoz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1cjehb9</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Nails by me @CandyCoated Claws 🍭💅🏻</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjehb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1cje4wd</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Is there a difference between jelly gel and sheer gel?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cje4wd/is_there_a_difference_between_jelly_gel_and_sheer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1cje0h6</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Does this colour suite me??</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjgfpp0bv8yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1cjdjqf</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Did my nails in cow print yesterday 🐮 🐄</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/upqxn3iur8yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1cjcn9x</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>My first successful ombre 🎉 only used two colors! Pink -&gt; Yellow</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjcn9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1cjc9ax</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Obsessed!</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4wwvjrbi8yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1cjbsb0</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Yaasss</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjbsb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1cjbryh</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>This might be my best mani</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1aidmlsge8yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1cjbo2e</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Sculpted Gel</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72z6g2rvd8yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1cjbn26</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>just painted em</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cjbn26/just_painted_em/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1cjb3fi</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Did gel nails with eye shadow. Had anyone tried this hack?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/liw2jt3b98yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1cja995</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Dip powder</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cja995/dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1cja8o9</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>April showers bring May flowers 🌸</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ng0nga7538yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1cja7mw</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>1st time trying sculpted nails</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lar49ww28yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1cj9zp2</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Sparkle sparkle</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypisu8w718yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1cj9wnt</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Best tool to use for shortening &amp; shaping press-ons?</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cj9wnt/best_tool_to_use_for_shortening_shaping_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1cj9l13</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Any tips on how to do Aquarium Nails properly?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cj9l13/any_tips_on_how_to_do_aquarium_nails_properly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1cj9i5v</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Dress matched set - u/creaturisms</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj9i5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1cj9feg</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>to die for</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g4erwyfxw7yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1cj9723</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Dress matched set - u/ElleElore</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj9723</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1cj8x66</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>I think this shape suits me but would love ideas [f28]</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kibmqyjzs7yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1cj8bw8</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>First time doing glitter ☺️</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj8bw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1cj8761</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Gel at Home: Tell me what I’m doing wrong</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cj8761/gel_at_home_tell_me_what_im_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1cj7l7r</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Can you share photos of your infills changing the design? An old acquaintance had an amazing tech who did some amazing transitions during infills and I'm kinda obsessed.</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cj7l7r/can_you_share_photos_of_your_infills_changing_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1cj6wgn</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Birthday Nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj6wgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1cj6las</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Best way to take off acrylics at home?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cj6las/best_way_to_take_off_acrylics_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1cj65ht</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So pretty in the light </t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w8iyg92w37yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1cj5mwf</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Does this colour clash with my skin tone?</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj5mwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1cj50lg</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Two weeks to grow out my nails</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj50lg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1ciz93i</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>New set.</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l3douowtv4yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1cjswqp</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What am I missing? </t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjswqp/what_am_i_missing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1cjsuoc</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Ever do nail art...</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjsuoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1cjs3vn</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>rate your brands by smell?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjs3vn/rate_your_brands_by_smell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1cjrapr</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Cadillacquer - Many Moons</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjrapr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1cjr3a4</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>ILNP - Flower Child</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l3eijgd1zbyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1cjqi72</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>These where my boyfriend's first unsupervised nails and wants an honest opinion.</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjg8wpz2tbyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1cjq32f</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pre-Mooncat </t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uzj5x5i1pbyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1cjpuil</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Cirque Lucky Bag, first time ordering and pleasantly surprised!</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjzd3lfqmbyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1cjl8gl</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Thistle Do Nicely</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpz3046ygayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1cjopi3</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Where am I going wrong n with my nail shape? Builder gel</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjopi3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1cjncu3</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>That girl we all know and love ❤️</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjncu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1cjmnuo</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Cool toned version of OPI Big Apple Red?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjmnuo/cool_toned_version_of_opi_big_apple_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1cjllno</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>velociraptor by mooncat 🦖</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b10i4xbxjayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1cjle18</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>How? Just hoooowwww?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f73k06b8iayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1cjl7vh</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>For a beginner is it easier to use the small (135mm) or large (195mm) glass file?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjl7vh/for_a_beginner_is_it_easier_to_use_the_small/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1cjkox1</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Drugstore polish can look excellent with the right application</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5ajoo7kcayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1cjkn0d</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>First Emily de Molly!</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjkn0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1cjkjsg</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>May The 4th be with you</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjkjsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1cjka51</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Ivy - Phoenix (PR Sample)</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjka51</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1cjk43b</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Do not buy from nailtiques.com !</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjk43b/do_not_buy_from_nailtiquescom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1cjjyqt</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Faberge Eggs Pahlish Mystery Bay Tree, Winter and Lilies of the Valley</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjjyqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1cjj37l</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Flakies never fail to amaze!</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/is378m330ayc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1cjj13f</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>With or without topper?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjj13f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1cjikfk</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Can't say no to a magnetic polish with strong contrasting colors</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjikfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1cjijic</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Time between base coat and color</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjijic/time_between_base_coat_and_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1cjh9c5</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Drugstore Top Coat for Swatch Sticks?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjh9c5/drugstore_top_coat_for_swatch_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1cjh03h</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Multichrome Flakies 💜 </t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjh03h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1cjg18x</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Simple nail art ideas?</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjg18x/simple_nail_art_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1cjcw9t</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Why do I always think water marbling will be fine</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h8hqmo2n8yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1cjekvp</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>The purpliest purple!</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjekvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1cjekq5</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Flakey Lubu Heels?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjekq5/flakey_lubu_heels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1cjeakq</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>I don’t think this beautiful polish even needs an intro 💚</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpt9kokdx8yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1cje85g</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>I just launched Daisy Chain Polish and here is my favorite color! (my brand)</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yh96zmnnw8yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1cjdxts</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Need help finding Anne Hathaway's polish!</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjdxts/need_help_finding_anne_hathaways_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1cjdx2o</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>It’s On by Wildflower Lacquer</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjdx2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1cjdhgo</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Valley Girl IS that girl</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjdhgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1cjcw0j</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>US made alternative to JelloJello peeling base gel?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjcw0j/us_made_alternative_to_jellojello_peeling_base_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1cjcrhk</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>magic 8 ball nails for my 18th bday!!</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjcrhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1cjcnin</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Psychedelic Zombie</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjcnin</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1cjcbhh</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Some ILNP Opal Sunset</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjcbhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1cjbo38</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Holo Taco Hi-Def dupes?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cjbo38/holo_taco_hidef_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1cjbghf</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Is there a shade similar to this? :not my photo, not my nails:</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5855qiac8yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1cjb38d</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Snow Cap - Polished for Days </t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjb38d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1cjahtq</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This polish looks so much nicer on the nail than it does in the bottle </t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjahtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1cja424</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Simple butterfly silhouettes!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cja424</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1cj9xcj</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>It's really grown on me!!</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj9xcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1cj9n73</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>⚠️💚Beware OGRE💚⚠️</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj9n73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1cj97nc</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Finally have a phone that takes good nail photos!</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkga2k8av7yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1cj92lv</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>ilnp petals vs mooncat spaceoddity?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cj92lv/ilnp_petals_vs_mooncat_spaceoddity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1cj8v3z</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Replacement brushes available in the UK?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cj8v3z/replacement_brushes_available_in_the_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1cj8uy9</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Blooming Azalea</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cj8uy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1cj7eby</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Y’all made me do it</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjoqe4qsf7yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1cj6jw1</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Help me!!!</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhzuj10y77yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1cj5l2k</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>My favorite red everrr!</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwexx7q0y6yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1cj4srp</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Poop 💩 Inspired/Named Polishes</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cj4srp/poop_inspirednamed_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1cjql0s</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Practicing my nail art skills 🙈</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjql0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1cjoz9w</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Little gift to myself for vacay 😊</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ydawbfaebyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1cjlhm8</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Loved my first try so much &gt;I&lt; did my hands. Im proud of them! My official second time doing nails :P Artist: me</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjlhm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1cjl1h3</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Recreated a Studio Ghibli set</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5ah3gsdfayc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1cjg4ag</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>one of the jobs that cost me the most but I loved it 😍</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcuiql22b9yc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1cjg30h</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art (last photo is what I was aiming for) (repost with credit)</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjg30h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1cjg29k</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Which nails would you pick?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/48sncckna9yc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1cjfteh</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>set on my lil sis</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjfteh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1cjd1vm</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Help! Is there a US made alternative to JelloJello peeling base gel? info in comments.... Bonus: here are some 3d bubble nails that I did on myself.</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6jo2wtin8yc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1cjbm16</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Pink and sparkles</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjbm16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1cjafcl</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>What do you think of this design?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0o2v2iaj48yc1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun May  5 08:07:35 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_05.xlsx
+++ b/data/2024_05_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1064"/>
+  <dimension ref="A1:C1215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18521,6 +18521,2573 @@
         </is>
       </c>
     </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ckm8fm</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Need some advice as a dude getting his nails done for the first time</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ckm8fm/need_some_advice_as_a_dude_getting_his_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1cklxuq</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Nail polish</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cklxuq/nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ckl706</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Broken toe nail, OK to fix with acrylic? </t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ckl706/broken_toe_nail_ok_to_fix_with_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ckkwal</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Extremely sloppy but I feel like it’s not bad for my very first try 🥴</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emn9zin1yjyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ckkqgt</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Made my first two sets of press ons! (regular nail polish)</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckkqgt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ckkiul</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>🖤🥰</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckkiul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1ckk3t3</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Turquoise cat eyes. </t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4vbs51cgojyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1ckjwac</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Almond nails on short, chubby fingies ft. doggo 🩷🩵🐶</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smxt5efzljyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1ckipnl</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Stained Glass Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckipnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1ckj7m1</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Gelx shine?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bo4hyjz4ejyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1ckhtu1</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Sentimental value &gt; Beauty</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckhtu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1ckhppq</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Unhappy with my new nails. Looking for advice?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckhppq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1ckhlek</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>May the 4th be with you</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckhlek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1ckhh4g</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Did my nails today 🤍</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drg19eogviyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1ckhbrd</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Engagement photo nails 💅💍</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gc3vmddxtiyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1ckha8p</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Short nails</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sy29858htiyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1ckaj6b</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>I love this shade, blue with glitter gel nails</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckaj6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1ck82zh</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Nails by IG: @marynnailz</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck82zh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1ck8r8f</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>What I got vs what I asked for - inspo pic from maniology.com</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck8r8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1cke9op</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lisa Frank Inspired </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cke9op/lisa_frank_inspired/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1ckei72</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Rubber base – sticky texture?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ckei72/rubber_base_sticky_texture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1ckg2x9</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Simple gel manicure</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ea95k49qhiyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1ckfj0a</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>got these done for graduation</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckfj0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1ckfdaq</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Are structured manicures easy to DIY?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ckfdaq/are_structured_manicures_easy_to_diy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1ckf1ux</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Flower Power Pastels 🌸</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a67kaud08iyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1ckel26</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Pre-refill bare nails 3 months since the last refill (swipe for after pictures)</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckel26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1ckeeqk</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>That one time I let my nail tech have free range 🩷💚💜</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckeeqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1ckdvn8</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Fresh set ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cb48b1vrxhyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1ckdivb</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Emerald or Plumb? 🌲😈</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckdivb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1ckd4cw</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Help please:)</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ckd4cw/help_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1ckcu44</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Need advice on pressons. Do these look bad?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckcu44</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1ckcagz</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Chrome tips for summer 🪩</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckcagz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1ckc5uu</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>First time trying nail decals</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckc5uu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1ckbrct</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>She never misses….</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a5irax4nfhyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1ckbps0</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>First time doing builder gel overlay on my natural nails</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckbps0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1ckayb6</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>can you refill hard gel nails with acrylic?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ckayb6/can_you_refill_hard_gel_nails_with_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1ckaloq</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>New set for my mom!</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckaloq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1cka7vn</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strawberries </t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdca7ws23hyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1cka7pf</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>I’m in love again 😍🥰🫣</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xs57kb13hyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1cka588</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Angel set 👼🏻🩵 </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tt7jofoh2hyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1cka2gs</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>The new set 😊</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9q2uvtev1hyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1ck9rz0</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Not used to wear bright pink on my nails. Still adjusting and battling whether I should turn them red by adding sheer red polish on top</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck9rz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1ck9bj5</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Hi I'm a guy and by no means I care about my nails however one thing that bothers me is that my nail looks childish/ immature compared to most guys nails it's hard to explain buy yeah</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck9bj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1ck914k</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Check out the growth!</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck914k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1ck8ssm</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Natural nail progress!</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck8ssm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1cjz1vs</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommendation for short almond shape fake nails? UK based </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cjz1vs/recommendation_for_short_almond_shape_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1cjzimb</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Credit:simlynail instagram. Is this a simple or intricate design?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccr4vy5coeyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1ck312l</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Best nail glue?</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ck312l/best_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1ck3oj0</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Did hand sanitizer mess up my acrylics?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ck3oj0/did_hand_sanitizer_mess_up_my_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1ck5yfn</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>What is the shortest safe stiletto/almond length?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck5yfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1ck8jbd</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Made a friend today, which nails do you choose if you want to add a second colour?</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uu3wv49ppgyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1ck8e90</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Seashells 🐚</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ik10b1hkogyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1ck893n</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Sunflowers</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/475curkfngyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1ck87s9</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Current nails ♥️</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rh1tydg4ngyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1ck84tt</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>working on growing my natural nails with the help of @jackieeenailsss</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ox4p5v7imgyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1ck7r63</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>It's been so long since I last posted. Thought I'd post my two favourite sets from the year so far.</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck7r63</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1ck7nd9</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Powerful color , do you like it ?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/419yobpsigyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1ck7a9q</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>My nails 55 days later 🩷</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck7a9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ck77uq</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Simple black set</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2c1bxqkffgyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ck7677</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Anyone have a Beetles color chart?</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ck7677/anyone_have_a_beetles_color_chart/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ck6x98</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Fire!</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck6x98</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ck6f3c</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>First Attempt At Ombré</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck6f3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ck5r5y</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>My first client!</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck5r5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ck5jdy</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fresh nails for the week </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck5jdy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ck5e2w</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Buenas Tardes Amigo</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzzx7r0x0gyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ck4n0i</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>I always end up going back to blue 🩵</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck4n0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ck47n6</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Natural nail lifting</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck47n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ck41xz</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Gifts for girlfriend who likes to do her own nails?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ck41xz/gifts_for_girlfriend_who_likes_to_do_her_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ck3wfm</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Discussion</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck3wfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1ck3ge2</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>New Mani</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcp534uqlfyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ck2v66</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>My partner's new nails :)</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/p8yIwtT.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ck2jwx</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>💎💎💎</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck2jwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ck1zj1</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Can we normalize taking nail pics showcasing every finger?</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfg8gbez9fyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1ck1h5z</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat approved </t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iaflg6dq5fyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1ck08wv</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Recognise BIAB from Shellac?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ck08wv/recognise_biab_from_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1cjzm4o</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Drooling Patrick 😂</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2culc1apeyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1cjzlh5</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Started seeing a new nail tech</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjzlh5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1cjz3gu</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>My Current Set</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbxj9h6dkeyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1cjz3e6</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Questions re: fills</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cjz3e6/questions_re_fills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1cjyiwy</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Does this colour look ok or is it too mustardy?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjyiwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1cjxpx8</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first artistic set diy </t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi82c00y5eyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1cjx9bh</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>The shape is not the best, but I love It. 🩷🌸</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjx9bh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1cjwneq</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh Set 😍 sheer matte with glossy hearts </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kib6p79ssdyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1cjwk9q</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Happy Star Wars day!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjwk9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1cjwbiw</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Milky mint</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n56texcgodyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1cjvhgs</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>DIY exgel nails</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjvhgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1cjvcls</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This jelly-like 🍬pink </t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhz6whyvbdyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1ckloon</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>The GLOW</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckloon</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1cklgl0</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Soft pink forever</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cklgl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ckhwsj</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Am I being too critical? Unhappy with my acrylic nails</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckhwsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1ckhsk5</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Finally got a peely base to last more than 24 hours!</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tq02dc5syiyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1ckhq7e</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I cannot stop staring </t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6jmswdj3yiyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ckh91m</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>caught in the rain 🌧️</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/131bq6o5tiyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1ckh3b9</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Wearing my homemade nail polish</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckh3b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1ckg0el</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Chibi-Chibi by Phoenix</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvt7rfu1hiyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1ckfmqx</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>What are your least favorite mooncat polishes and why?</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ckfmqx/what_are_your_least_favorite_mooncat_polishes_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1ckfjoo</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>I just got an order from Parrot Polish</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77xm831mciyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1ckezmk</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Flower Power Pastels</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c70gsd8h7iyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1ckdxbt</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>First time trying press ons 🥹</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hq1kuew6yhyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1ckdsfv</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hate the formula, love the colour </t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ewqxpuzwhyc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1ckdnpn</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Oh la la. Finally tried a French tip on my favorite nail shape.</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68st9l4tvhyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1ckdjih</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>ILNP “Flower child”</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckdjih</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1ckcmw8</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>best way to stop biting your nails when you have tried EVERYTHING?</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ckcmw8/best_way_to_stop_biting_your_nails_when_you_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1ckcfjs</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Is it harmful to paint my nails in a very small room?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ckcfjs/is_it_harmful_to_paint_my_nails_in_a_very_small/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1ckbkxc</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>What’s your favorite maroon?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ckbkxc/whats_your_favorite_maroon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1ckaaxe</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Lagoon + Sea</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2o285ns3hyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1ckaa8k</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Not perfect but I'm actually quite happy with how this turned out!</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/35h33jdm3hyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1ck9zoo</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Let's hit the beach when it's 70° and overcast</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0xlhn431hyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1ck9qdc</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>ILNP Lily</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck9qdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1ck9881</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Harbour Island 🩵</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck9881</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1ck8rvb</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Flicker by ILNP is such a cozy grey. Looks like a candle or bonfire is reflecting on your nails 🕯️</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck8rvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1ck862d</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>first ppu order came in!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0u6y5dqrmgyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1ck7nux</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Mandalorian Nails for May the 4th! 🚀</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck7nux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1ck7gxj</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Removing chunky glitter</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unz1fthfhgyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1ck776v</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>nail tech filed down to my nail bed</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck776v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1ck6k4j</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Some Recent Favourites</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck6k4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1ck6jfw</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Ghost Rose</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck6jfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1ck6cev</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Let it bee</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck6cev</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1ck5s9k</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>🌱 Thistle and Thorn 🌱</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck5s9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ck5ft6</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>In the rain, no flash or filters, just GLOW</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck5ft6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1ck51vt</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Reds always look bad on me, but this one is just.. 😍</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imit4es6yfyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1ck4lad</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Inside Job is now my favorite</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck4lad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1ck4kw7</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>When you buy something you think is different....</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck4kw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1ck4god</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>How can I clean builder gel off of pots and ziplock bags?</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ck4god/how_can_i_clean_builder_gel_off_of_pots_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1ck467o</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Recent ones</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck467o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1ck3pak</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Spring drugstore nails</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck3pak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1ck2wrz</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Best UV LED Curing Lamp?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ck2wrz/best_uv_led_curing_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1ck1wxg</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Palette London Pearl Top Coat</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ck1wxg/palette_london_pearl_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1ck1zao</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Finally decided to attempt velvet nails</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b83c292x9fyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1ck1t45</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>I just bought a gorgeous pink glow in the dark polish- need a blue one now</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ck1t45/i_just_bought_a_gorgeous_pink_glow_in_the_dark/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1ck1lh3</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>boobies in the wild 👀</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mht0z0ar6fyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1ck0rq5</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>May the 4th nails</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3nw839cszeyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1ck0ex7</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Zoya India, she's so pretty 😍</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck0ex7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1cjyip7</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>🌌May the Fourth🌌</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjyip7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1cjxtev</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>A DIY colour</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5f27ztn07eyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1cjwtad</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>First time doing gel nails at home was a success 🥹🌸</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3j0blpxudyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1cjst7d</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Cupcake Lilac Skies</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0bp5jk1hcyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1ckl73i</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Doja Cat Inspired Press On Nails! 🕷❤️</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gll2316p1kyc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1ckjhxn</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Lumpy space princess x Kirby</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofk2r9afhjyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1ckjfm1</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>This is my first time doing the moon crescent on press ons.</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckjfm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1ckh7es</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>first time i try to draw stars</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1okdmstnsiyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1cke8cw</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Currently obsessed with 3d 🥞 </t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cke8cw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1ckdtzb</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Studio Ghibli nail art</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckdtzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1ckc8bo</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome tips for summer 🪩 </t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ckc8bo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1ck8296</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Nails by IG: @marynnailz</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ck8296</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1ck4zvc</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>first three sets ever</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfjzwe0sxfyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1ck4q16</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>nail art advice needed</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ck4q16/nail_art_advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1ck4oav</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>swirl jelly nails</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g26ihyh6vfyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1ck2w0p</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>My partner's new nails :)</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/p8yIwtT.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1ck0i1u</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>A gift for a friend 💙</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxqd2taaxeyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1cjw0dj</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Wavey line art is my go to lately, anyone else? 💜</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cjw0dj</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>